<commit_message>
sheet updated, and prblms
</commit_message>
<xml_diff>
--- a/dsa-track-sheet/DSA-tracksheet.xlsx
+++ b/dsa-track-sheet/DSA-tracksheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dsa-work\DSA\dsa-track-sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D31F52-007F-41AC-ADF1-AD254B9818C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB123D1-4067-4463-8D78-2D79AA34564E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ACC6A297-66BE-4056-8F0D-CD389159DB30}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{ACC6A297-66BE-4056-8F0D-CD389159DB30}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Target" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="256">
   <si>
     <t>Topic</t>
   </si>
@@ -717,6 +717,113 @@
   </si>
   <si>
     <t>IF not reason</t>
+  </si>
+  <si>
+    <t>Palindrome Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/palindrome-number/description/</t>
+  </si>
+  <si>
+    <t>Convert integer into String and check each char by 2 pointer</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/roman-to-integer/description/</t>
+  </si>
+  <si>
+    <t>Roman To Integer</t>
+  </si>
+  <si>
+    <t>Iterate String in reverse and  check prev element with current if current is greater then minus it and save as ans</t>
+  </si>
+  <si>
+    <t>get power of each digit and sum for both the string and again convert that sum into binary</t>
+  </si>
+  <si>
+    <t>Not working for large input</t>
+  </si>
+  <si>
+    <t>Bin Manupulation</t>
+  </si>
+  <si>
+    <t>Counting Bits</t>
+  </si>
+  <si>
+    <t>Number of 1 bits</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/counting-bits/description/</t>
+  </si>
+  <si>
+    <t>If number is even so number of bits will be same as half of  number bits 
+ex - 18 number of bits will be same as 9
+and If number is odd then number of bits of previous number + 1</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/number-of-1-bits/</t>
+  </si>
+  <si>
+    <t>take count variable and update if number reminder is 1 with 2 and divide the number by 2</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/single-number/description/</t>
+  </si>
+  <si>
+    <t>check i with i+1 and compare if both r not equal then return the array of i</t>
+  </si>
+  <si>
+    <t>xOr (^) operator is not clear fully</t>
+  </si>
+  <si>
+    <t>Missing Number</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/missing-number/description/</t>
+  </si>
+  <si>
+    <t>Ransom Note</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/ransom-note/description/</t>
+  </si>
+  <si>
+    <t>HashTable</t>
+  </si>
+  <si>
+    <t>Used hashMap</t>
+  </si>
+  <si>
+    <t>5 question</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Occupied in ofc work</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Outside of home (ujjain)</t>
+  </si>
+  <si>
+    <t>Occupied in house clining</t>
+  </si>
+  <si>
+    <t>Climbing Stairs</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/climbing-stairs/</t>
+  </si>
+  <si>
+    <t>memoize the result into result array and check if that exist then return from array else call recursion function</t>
   </si>
 </sst>
 </file>
@@ -938,10 +1045,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1257,10 +1364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B6EF23C-20FC-406F-ACE2-509B3A9D1D3C}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1271,10 +1378,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="34"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
@@ -1288,8 +1395,44 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="34">
+      <c r="A3" s="33">
         <v>45589</v>
+      </c>
+      <c r="B3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="33">
+        <v>45590</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="33">
+        <v>45591</v>
+      </c>
+      <c r="B5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="33">
+        <v>45592</v>
+      </c>
+      <c r="B6" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -1627,11 +1770,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6C3F20-9441-4363-A20B-E92D50539D47}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2241,9 +2384,15 @@
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="J20" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K20" s="4">
+        <v>45590</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -2870,6 +3019,8 @@
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
@@ -2900,6 +3051,256 @@
       <c r="J41" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" s="4">
+        <v>45589</v>
+      </c>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G43" s="4">
+        <v>45589</v>
+      </c>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+    </row>
+    <row r="44" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C44" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="4">
+        <v>45590</v>
+      </c>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J44" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G45" s="4">
+        <v>45590</v>
+      </c>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C46" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G46" s="4">
+        <v>45590</v>
+      </c>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C47" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G47" s="4">
+        <v>45590</v>
+      </c>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G48" s="4">
+        <v>45590</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G49" s="4">
+        <v>45593</v>
+      </c>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2934,18 +3335,26 @@
     <hyperlink ref="B36" r:id="rId29" xr:uid="{DBEF156F-46E7-4ABC-BD7D-07B3C0726238}"/>
     <hyperlink ref="B37" r:id="rId30" xr:uid="{D5D353B3-CFB8-49DD-A37B-4B9BE8A8E9A1}"/>
     <hyperlink ref="B38" r:id="rId31" xr:uid="{98574129-D3D4-4BD0-B3D8-2DC8F1C81177}"/>
+    <hyperlink ref="B43" r:id="rId32" xr:uid="{18F4D5FD-E962-477E-B72C-01998BC81735}"/>
+    <hyperlink ref="B44" r:id="rId33" xr:uid="{1015FAEE-E16E-49C3-A0EF-7A6AF90C60A2}"/>
+    <hyperlink ref="B45" r:id="rId34" xr:uid="{D51FB25A-0C2A-4ED6-BC14-E335FF4A3DBD}"/>
+    <hyperlink ref="B46" r:id="rId35" xr:uid="{0E2E5755-8934-433D-8938-2A2CD39610D0}"/>
+    <hyperlink ref="B47" r:id="rId36" xr:uid="{AEA4AC34-1730-412B-BAE4-FA5276A74215}"/>
+    <hyperlink ref="B48" r:id="rId37" xr:uid="{88CCBA4A-3DB5-4214-A612-FB365913C42E}"/>
+    <hyperlink ref="B49" r:id="rId38" xr:uid="{FCFABEF0-D398-4734-9490-622554354EC0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId32"/>
+  <pageSetup orientation="portrait" r:id="rId39"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C68BFB48-6237-44A1-BCC7-17106A42F822}">
-  <dimension ref="A2:D31"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2956,23 +3365,37 @@
     <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>5</v>
+      <c r="A2" s="25">
+        <v>45559</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="25">
-        <v>45559</v>
+        <v>45560</v>
       </c>
       <c r="B3" s="25" t="s">
         <v>73</v>
@@ -2981,110 +3404,110 @@
         <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="25">
-        <v>45560</v>
+        <v>45561</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="25">
-        <v>45561</v>
+        <v>45562</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="25">
-        <v>45562</v>
+        <v>45563</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="25">
-        <v>45563</v>
+        <v>45564</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="25">
-        <v>45564</v>
+        <v>45567</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>119</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="25">
-        <v>45567</v>
+        <v>45568</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="25">
-        <v>45568</v>
+        <v>45569</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="25">
-        <v>45569</v>
+        <v>45570</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>99</v>
@@ -3098,24 +3521,24 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="25">
-        <v>45570</v>
+        <v>45571</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="25">
-        <v>45571</v>
+        <v>45572</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>99</v>
+        <v>158</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>137</v>
@@ -3126,41 +3549,41 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="25">
-        <v>45572</v>
+        <v>45573</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>158</v>
+        <v>73</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>137</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="25">
-        <v>45573</v>
+        <v>45574</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>73</v>
+        <v>119</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="25">
-        <v>45574</v>
+        <v>45575</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>119</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>121</v>
@@ -3168,7 +3591,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="25">
-        <v>45575</v>
+        <v>45576</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>119</v>
@@ -3185,18 +3608,18 @@
         <v>45576</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>160</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="25">
-        <v>45576</v>
+        <v>45577</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>99</v>
@@ -3210,7 +3633,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="25">
-        <v>45577</v>
+        <v>45578</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>99</v>
@@ -3224,13 +3647,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="25">
-        <v>45578</v>
+        <v>45579</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>135</v>
@@ -3238,13 +3661,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="25">
-        <v>45579</v>
+        <v>45580</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>73</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>135</v>
@@ -3252,35 +3675,35 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="25">
-        <v>45580</v>
+        <v>45581</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="25">
-        <v>45581</v>
+        <v>45582</v>
       </c>
       <c r="B24" s="25" t="s">
-        <v>180</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="25">
-        <v>45582</v>
+        <v>45583</v>
       </c>
       <c r="B25" s="25" t="s">
         <v>73</v>
@@ -3294,21 +3717,21 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="25">
-        <v>45583</v>
+        <v>45584</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>73</v>
+        <v>180</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="25">
-        <v>45584</v>
+        <v>45585</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>180</v>
@@ -3322,21 +3745,21 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="25">
-        <v>45585</v>
+        <v>45586</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="25">
-        <v>45586</v>
+        <v>45587</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>99</v>
@@ -3350,7 +3773,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="25">
-        <v>45587</v>
+        <v>45588</v>
       </c>
       <c r="B30" s="25" t="s">
         <v>99</v>
@@ -3364,16 +3787,58 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="25">
-        <v>45588</v>
+        <v>45589</v>
       </c>
       <c r="B31" s="25" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
+        <v>45590</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
+        <v>45591</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
+        <v>45592</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3387,7 +3852,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,7 +3977,9 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+      <c r="A13" s="11" t="s">
+        <v>239</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>